<commit_message>
update biorefineries for new biosteam version; update docs; enhancements to cornstover; implement agile biorefinery for sugarcane 2g; more work on lipidcane 2g
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane/results/Monte Carlo across lipid fraction.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane/results/Monte Carlo across lipid fraction.xlsx
@@ -507,124 +507,124 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.1266519392190363</v>
+        <v>0.1263771079727516</v>
       </c>
       <c r="C2">
-        <v>0.1320827987746284</v>
+        <v>0.131882303219976</v>
       </c>
       <c r="D2">
-        <v>0.1365222240669869</v>
+        <v>0.1364141541486866</v>
       </c>
       <c r="E2">
-        <v>0.1406062527077547</v>
+        <v>0.1405941358863532</v>
       </c>
       <c r="F2">
-        <v>0.1445717958305068</v>
+        <v>0.1446569484277321</v>
       </c>
       <c r="G2">
-        <v>0.1483073852737691</v>
+        <v>0.1485416934058388</v>
       </c>
       <c r="H2">
-        <v>0.1521789089213643</v>
+        <v>0.1524966505124935</v>
       </c>
       <c r="I2">
-        <v>0.1565247998166276</v>
+        <v>0.1569294417113175</v>
       </c>
       <c r="J2">
-        <v>0.1602933860625438</v>
+        <v>0.1607816384629603</v>
       </c>
       <c r="K2">
-        <v>0.1637539748537611</v>
+        <v>0.1643302040077098</v>
       </c>
       <c r="L2">
-        <v>0.1674132316854152</v>
+        <v>0.1680385073982598</v>
       </c>
       <c r="M2">
-        <v>0.1702778475764708</v>
+        <v>0.1709874227734602</v>
       </c>
       <c r="N2">
-        <v>0.1731075043641316</v>
+        <v>0.1739025735896073</v>
       </c>
       <c r="O2">
-        <v>0.1759031031281533</v>
+        <v>0.1767846392578043</v>
       </c>
       <c r="P2">
-        <v>0.1786605609958584</v>
+        <v>0.1796337816898061</v>
       </c>
       <c r="Q2">
-        <v>0.1813936421817675</v>
+        <v>0.1824555786624679</v>
       </c>
       <c r="R2">
-        <v>0.1840950490928017</v>
+        <v>0.1852468843540655</v>
       </c>
       <c r="S2">
-        <v>0.1867309204485328</v>
+        <v>0.1879817717515009</v>
       </c>
       <c r="T2">
-        <v>0.1893740636906069</v>
+        <v>0.1907174567173378</v>
       </c>
       <c r="U2">
-        <v>0.1919640353803449</v>
+        <v>0.1934013512792702</v>
       </c>
       <c r="V2">
-        <v>0.1945524316079204</v>
+        <v>0.1960853859550391</v>
       </c>
       <c r="W2">
-        <v>0.1971680013594136</v>
+        <v>0.1987841472119619</v>
       </c>
       <c r="X2">
-        <v>0.1984594698112844</v>
+        <v>0.2001788398985246</v>
       </c>
       <c r="Y2">
-        <v>0.2019453033801686</v>
+        <v>0.2037646769751738</v>
       </c>
       <c r="Z2">
-        <v>0.2034934617698277</v>
+        <v>0.2054157924359034</v>
       </c>
       <c r="AA2">
-        <v>0.2068844039925832</v>
+        <v>0.2089159433379385</v>
       </c>
       <c r="AB2">
-        <v>0.2084023352719326</v>
+        <v>0.2105441536243976</v>
       </c>
       <c r="AC2">
-        <v>0.2117632894698791</v>
+        <v>0.2140120079238091</v>
       </c>
       <c r="AD2">
-        <v>0.2132597954658697</v>
+        <v>0.215619203768213</v>
       </c>
       <c r="AE2">
-        <v>0.2156410528349181</v>
+        <v>0.2181191135127548</v>
       </c>
       <c r="AF2">
-        <v>0.2180250813730967</v>
+        <v>0.2206170377220371</v>
       </c>
       <c r="AG2">
-        <v>0.22039950124457</v>
+        <v>0.2231031836858132</v>
       </c>
       <c r="AH2">
-        <v>0.2226763231244384</v>
+        <v>0.2255131861274797</v>
       </c>
       <c r="AI2">
-        <v>0.224880919839477</v>
+        <v>0.2278718614193154</v>
       </c>
       <c r="AJ2">
-        <v>0.227124379360835</v>
+        <v>0.2302570813832683</v>
       </c>
       <c r="AK2">
-        <v>0.2294469244436002</v>
+        <v>0.2327028854575225</v>
       </c>
       <c r="AL2">
-        <v>0.2316686852283727</v>
+        <v>0.23507120182545</v>
       </c>
       <c r="AM2">
-        <v>0.2338019887070642</v>
+        <v>0.2373724673852868</v>
       </c>
       <c r="AN2">
-        <v>0.2354125033221247</v>
+        <v>0.2392735549595764</v>
       </c>
       <c r="AO2">
-        <v>0.2383037468790247</v>
+        <v>0.2421459389766333</v>
       </c>
     </row>
   </sheetData>
@@ -767,124 +767,124 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4594933.690626844</v>
+        <v>4596739.77870624</v>
       </c>
       <c r="C2">
-        <v>6108293.198692793</v>
+        <v>6110121.35726426</v>
       </c>
       <c r="D2">
-        <v>7605036.044132697</v>
+        <v>7606441.948604696</v>
       </c>
       <c r="E2">
-        <v>9058508.365223253</v>
+        <v>9059112.278045349</v>
       </c>
       <c r="F2">
-        <v>10466855.05468448</v>
+        <v>10466300.66817262</v>
       </c>
       <c r="G2">
-        <v>11832657.09581897</v>
+        <v>11829857.90282767</v>
       </c>
       <c r="H2">
-        <v>13151702.24317585</v>
+        <v>13147242.59904813</v>
       </c>
       <c r="I2">
-        <v>14417986.89457383</v>
+        <v>14411589.69478941</v>
       </c>
       <c r="J2">
-        <v>15650246.40858212</v>
+        <v>15641699.57535029</v>
       </c>
       <c r="K2">
-        <v>16863990.44220488</v>
+        <v>16852969.30223284</v>
       </c>
       <c r="L2">
-        <v>18058375.0341168</v>
+        <v>18044614.65778005</v>
       </c>
       <c r="M2">
-        <v>19234442.86174945</v>
+        <v>19217681.83891526</v>
       </c>
       <c r="N2">
-        <v>20379429.33247763</v>
+        <v>20359409.33537341</v>
       </c>
       <c r="O2">
-        <v>21493981.92079541</v>
+        <v>21470454.34025065</v>
       </c>
       <c r="P2">
-        <v>22578808.22429512</v>
+        <v>22551403.7177843</v>
       </c>
       <c r="Q2">
-        <v>23634224.05829557</v>
+        <v>23602813.10777451</v>
       </c>
       <c r="R2">
-        <v>24661032.0557407</v>
+        <v>24625371.14144303</v>
       </c>
       <c r="S2">
-        <v>25660939.84227562</v>
+        <v>25620513.37289041</v>
       </c>
       <c r="T2">
-        <v>26632186.85268205</v>
+        <v>26587012.36507841</v>
       </c>
       <c r="U2">
-        <v>27577363.12671858</v>
+        <v>27527187.50014611</v>
       </c>
       <c r="V2">
-        <v>28495216.94969535</v>
+        <v>28439798.48891104</v>
       </c>
       <c r="W2">
-        <v>29385092.89277413</v>
+        <v>29324744.62747439</v>
       </c>
       <c r="X2">
-        <v>30368299.84383385</v>
+        <v>30301514.54925343</v>
       </c>
       <c r="Y2">
-        <v>31119186.84031079</v>
+        <v>31046872.85277091</v>
       </c>
       <c r="Z2">
-        <v>32030717.45205331</v>
+        <v>31951658.44733849</v>
       </c>
       <c r="AA2">
-        <v>32730951.74605981</v>
+        <v>32645670.93145756</v>
       </c>
       <c r="AB2">
-        <v>33597815.51684737</v>
+        <v>33505046.46144887</v>
       </c>
       <c r="AC2">
-        <v>34246829.65820542</v>
+        <v>34147673.68989405</v>
       </c>
       <c r="AD2">
-        <v>35070362.33543289</v>
+        <v>34963285.49446175</v>
       </c>
       <c r="AE2">
-        <v>35773411.52461211</v>
+        <v>35658460.95466016</v>
       </c>
       <c r="AF2">
-        <v>36453491.55317312</v>
+        <v>36330737.90453882</v>
       </c>
       <c r="AG2">
-        <v>37111471.43472846</v>
+        <v>36980869.88035478</v>
       </c>
       <c r="AH2">
-        <v>37752172.49956214</v>
+        <v>37612432.82078218</v>
       </c>
       <c r="AI2">
-        <v>38374903.17794525</v>
+        <v>38224726.11357758</v>
       </c>
       <c r="AJ2">
-        <v>38974486.8919296</v>
+        <v>38814342.93301651</v>
       </c>
       <c r="AK2">
-        <v>39548869.74824516</v>
+        <v>39379650.94548032</v>
       </c>
       <c r="AL2">
-        <v>40107985.12988172</v>
+        <v>39928210.02851827</v>
       </c>
       <c r="AM2">
-        <v>40651712.61869876</v>
+        <v>40459949.66194697</v>
       </c>
       <c r="AN2">
-        <v>41205507.546984</v>
+        <v>40994090.39055227</v>
       </c>
       <c r="AO2">
-        <v>41687041.0706769</v>
+        <v>41474696.2704834</v>
       </c>
     </row>
   </sheetData>
@@ -1027,124 +1027,124 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>60064119.54857426</v>
+        <v>60087728.39640974</v>
       </c>
       <c r="C2">
-        <v>58172405.58427875</v>
+        <v>58189816.07497269</v>
       </c>
       <c r="D2">
-        <v>56221083.5648373</v>
+        <v>56231476.87163371</v>
       </c>
       <c r="E2">
-        <v>54301520.18853938</v>
+        <v>54305140.36340471</v>
       </c>
       <c r="F2">
-        <v>52422171.44788102</v>
+        <v>52419394.85982081</v>
       </c>
       <c r="G2">
-        <v>50594832.68867061</v>
+        <v>50582863.72008553</v>
       </c>
       <c r="H2">
-        <v>48797110.1712029</v>
+        <v>48780563.43513779</v>
       </c>
       <c r="I2">
-        <v>47010416.31437303</v>
+        <v>46989557.99154954</v>
       </c>
       <c r="J2">
-        <v>45296023.52208097</v>
+        <v>45271286.68733718</v>
       </c>
       <c r="K2">
-        <v>43681628.61535363</v>
+        <v>43653081.31838816</v>
       </c>
       <c r="L2">
-        <v>42144752.27564506</v>
+        <v>42112638.22048581</v>
       </c>
       <c r="M2">
-        <v>40673600.03317403</v>
+        <v>40638156.78463261</v>
       </c>
       <c r="N2">
-        <v>39232796.44285362</v>
+        <v>39194255.59569041</v>
       </c>
       <c r="O2">
-        <v>37821756.03533212</v>
+        <v>37780355.86970694</v>
       </c>
       <c r="P2">
-        <v>36440022.70621701</v>
+        <v>36395794.47106894</v>
       </c>
       <c r="Q2">
-        <v>35086553.67859639</v>
+        <v>35039922.06510087</v>
       </c>
       <c r="R2">
-        <v>33761147.77417125</v>
+        <v>33712327.70067861</v>
       </c>
       <c r="S2">
-        <v>32464680.29794466</v>
+        <v>32413535.15625334</v>
       </c>
       <c r="T2">
-        <v>31193567.30450601</v>
+        <v>31140655.63685717</v>
       </c>
       <c r="U2">
-        <v>29949832.3814414</v>
+        <v>29895340.16626571</v>
       </c>
       <c r="V2">
-        <v>28730957.82530956</v>
+        <v>28675080.8877046</v>
       </c>
       <c r="W2">
-        <v>27535552.42774275</v>
+        <v>27479002.56999182</v>
       </c>
       <c r="X2">
-        <v>26232146.00579101</v>
+        <v>26174456.84941801</v>
       </c>
       <c r="Y2">
-        <v>25186404.72741845</v>
+        <v>25127877.190469</v>
       </c>
       <c r="Z2">
-        <v>23961650.87809188</v>
+        <v>23902508.14197984</v>
       </c>
       <c r="AA2">
-        <v>22969384.73676992</v>
+        <v>22909537.78039474</v>
       </c>
       <c r="AB2">
-        <v>21788022.89990607</v>
+        <v>21727862.61054406</v>
       </c>
       <c r="AC2">
-        <v>20843667.19880188</v>
+        <v>20783317.84603306</v>
       </c>
       <c r="AD2">
-        <v>19704371.48543654</v>
+        <v>19644210.09241179</v>
       </c>
       <c r="AE2">
-        <v>18691941.16614508</v>
+        <v>18631878.42124644</v>
       </c>
       <c r="AF2">
-        <v>17704496.72663235</v>
+        <v>17644878.52607512</v>
       </c>
       <c r="AG2">
-        <v>16738081.67514794</v>
+        <v>16679177.53043213</v>
       </c>
       <c r="AH2">
-        <v>15794118.52304263</v>
+        <v>15735656.58819508</v>
       </c>
       <c r="AI2">
-        <v>14871447.09503443</v>
+        <v>14813248.89562073</v>
       </c>
       <c r="AJ2">
-        <v>13967478.37832547</v>
+        <v>13910086.80086249</v>
       </c>
       <c r="AK2">
-        <v>13081307.33306845</v>
+        <v>13025335.9948332</v>
       </c>
       <c r="AL2">
-        <v>12215915.50185178</v>
+        <v>12161160.38412445</v>
       </c>
       <c r="AM2">
-        <v>11370491.42503323</v>
+        <v>11316854.34765258</v>
       </c>
       <c r="AN2">
-        <v>10550859.16899032</v>
+        <v>10496724.83656216</v>
       </c>
       <c r="AO2">
-        <v>9735444.256638842</v>
+        <v>9685854.00239254</v>
       </c>
     </row>
   </sheetData>
@@ -1287,124 +1287,124 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>181923693.8199539</v>
+        <v>182211002.3322872</v>
       </c>
       <c r="C2">
-        <v>183330118.7505441</v>
+        <v>183531423.10008</v>
       </c>
       <c r="D2">
-        <v>184606334.6485538</v>
+        <v>184704111.6482563</v>
       </c>
       <c r="E2">
-        <v>185905739.8976079</v>
+        <v>185898136.3881662</v>
       </c>
       <c r="F2">
-        <v>187177905.8715034</v>
+        <v>187065217.6155345</v>
       </c>
       <c r="G2">
-        <v>188592918.2229369</v>
+        <v>188320470.3385141</v>
       </c>
       <c r="H2">
-        <v>189768622.2714101</v>
+        <v>189409640.3238878</v>
       </c>
       <c r="I2">
-        <v>190357211.9630381</v>
+        <v>189911542.2456904</v>
       </c>
       <c r="J2">
-        <v>191485040.3104586</v>
+        <v>190955795.4985475</v>
       </c>
       <c r="K2">
-        <v>192522833.0223612</v>
+        <v>191906398.6981884</v>
       </c>
       <c r="L2">
-        <v>192766690.6134627</v>
+        <v>192062767.8594966</v>
       </c>
       <c r="M2">
-        <v>193677445.5796002</v>
+        <v>192885698.4973143</v>
       </c>
       <c r="N2">
-        <v>194577473.4253535</v>
+        <v>193697525.6463881</v>
       </c>
       <c r="O2">
-        <v>195467460.7642194</v>
+        <v>194499166.5856293</v>
       </c>
       <c r="P2">
-        <v>196354250.9355755</v>
+        <v>195292848.5907481</v>
       </c>
       <c r="Q2">
-        <v>197223368.8869196</v>
+        <v>196073015.7618885</v>
       </c>
       <c r="R2">
-        <v>198084467.33198</v>
+        <v>196844760.9386395</v>
       </c>
       <c r="S2">
-        <v>198975319.971229</v>
+        <v>197637073.8578999</v>
       </c>
       <c r="T2">
-        <v>199818955.4675308</v>
+        <v>198390283.6310282</v>
       </c>
       <c r="U2">
-        <v>200681166.4458969</v>
+        <v>199161123.3715741</v>
       </c>
       <c r="V2">
-        <v>201508322.5578728</v>
+        <v>199896262.3018367</v>
       </c>
       <c r="W2">
-        <v>202271824.0418027</v>
+        <v>200582181.0197221</v>
       </c>
       <c r="X2">
-        <v>203019933.9388623</v>
+        <v>201225283.8442827</v>
       </c>
       <c r="Y2">
-        <v>203849374.2772988</v>
+        <v>201966090.8747699</v>
       </c>
       <c r="Z2">
-        <v>204605787.02141</v>
+        <v>202620453.5286523</v>
       </c>
       <c r="AA2">
-        <v>205456810.1909043</v>
+        <v>203374970.6143662</v>
       </c>
       <c r="AB2">
-        <v>206201235.8877421</v>
+        <v>204011128.1437108</v>
       </c>
       <c r="AC2">
-        <v>207007079.8955558</v>
+        <v>204725396.3408416</v>
       </c>
       <c r="AD2">
-        <v>207730765.1554207</v>
+        <v>205341780.580371</v>
       </c>
       <c r="AE2">
-        <v>208487114.66381</v>
+        <v>205989956.4207962</v>
       </c>
       <c r="AF2">
-        <v>209228162.127151</v>
+        <v>206628691.171212</v>
       </c>
       <c r="AG2">
-        <v>209953097.1241403</v>
+        <v>207254477.558488</v>
       </c>
       <c r="AH2">
-        <v>210750504.3433866</v>
+        <v>207930735.4785731</v>
       </c>
       <c r="AI2">
-        <v>211594917.9441565</v>
+        <v>208633186.6157412</v>
       </c>
       <c r="AJ2">
-        <v>212375362.373049</v>
+        <v>209285941.7907197</v>
       </c>
       <c r="AK2">
-        <v>213053786.007214</v>
+        <v>209857882.1235547</v>
       </c>
       <c r="AL2">
-        <v>213809136.4386926</v>
+        <v>210483010.5399592</v>
       </c>
       <c r="AM2">
-        <v>214629087.4975894</v>
+        <v>211151194.0779106</v>
       </c>
       <c r="AN2">
-        <v>215938820.917738</v>
+        <v>212178432.4130722</v>
       </c>
       <c r="AO2">
-        <v>215891712.6013346</v>
+        <v>212183588.0866981</v>
       </c>
     </row>
   </sheetData>
@@ -2073,13 +2073,13 @@
         <v>695643.488675155</v>
       </c>
       <c r="D2">
-        <v>688822.4568321186</v>
+        <v>688822.4568321184</v>
       </c>
       <c r="E2">
         <v>681652.5925288347</v>
       </c>
       <c r="F2">
-        <v>674404.9546450276</v>
+        <v>674404.9546450275</v>
       </c>
       <c r="G2">
         <v>667139.9343443163</v>
@@ -2091,37 +2091,37 @@
         <v>652601.2453604748</v>
       </c>
       <c r="J2">
-        <v>645331.2806944958</v>
+        <v>645331.280694496</v>
       </c>
       <c r="K2">
-        <v>641426.0426595397</v>
+        <v>641426.0426595398</v>
       </c>
       <c r="L2">
         <v>641904.2142798619</v>
       </c>
       <c r="M2">
-        <v>642382.3327764543</v>
+        <v>642382.3327764545</v>
       </c>
       <c r="N2">
         <v>642860.7925910689</v>
       </c>
       <c r="O2">
-        <v>643338.2541141367</v>
+        <v>643338.2541141368</v>
       </c>
       <c r="P2">
         <v>643816.0476071427</v>
       </c>
       <c r="Q2">
-        <v>644293.4445357942</v>
+        <v>644293.444535794</v>
       </c>
       <c r="R2">
         <v>644772.655339617</v>
       </c>
       <c r="S2">
-        <v>645249.3114351666</v>
+        <v>645249.3114351667</v>
       </c>
       <c r="T2">
-        <v>645726.7626781731</v>
+        <v>645726.7626781734</v>
       </c>
       <c r="U2">
         <v>646204.7046694835</v>
@@ -2133,19 +2133,19 @@
         <v>647161.806821914</v>
       </c>
       <c r="X2">
-        <v>647483.1938594318</v>
+        <v>647483.1938594319</v>
       </c>
       <c r="Y2">
-        <v>648066.4323788421</v>
+        <v>648066.432378842</v>
       </c>
       <c r="Z2">
-        <v>648434.8387509256</v>
+        <v>648434.8387509254</v>
       </c>
       <c r="AA2">
         <v>649027.0169198607</v>
       </c>
       <c r="AB2">
-        <v>649387.4016308555</v>
+        <v>649387.4016308556</v>
       </c>
       <c r="AC2">
         <v>649979.2192438802</v>
@@ -2157,13 +2157,13 @@
         <v>650811.2405310487</v>
       </c>
       <c r="AF2">
-        <v>651287.2117887659</v>
+        <v>651287.2117887657</v>
       </c>
       <c r="AG2">
         <v>651761.911104982</v>
       </c>
       <c r="AH2">
-        <v>652237.5098450603</v>
+        <v>652237.5098450602</v>
       </c>
       <c r="AI2">
         <v>652713.0557323</v>
@@ -2175,10 +2175,10 @@
         <v>653663.7695837953</v>
       </c>
       <c r="AL2">
-        <v>654139.2375250297</v>
+        <v>654139.2375250295</v>
       </c>
       <c r="AM2">
-        <v>654615.0421234925</v>
+        <v>654615.0421234922</v>
       </c>
       <c r="AN2">
         <v>655130.0935470394</v>
@@ -2327,124 +2327,124 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>48193.30980827774</v>
+        <v>48270.4795242657</v>
       </c>
       <c r="C2">
-        <v>48322.00128568195</v>
+        <v>48398.09421565657</v>
       </c>
       <c r="D2">
-        <v>48215.31637562352</v>
+        <v>48290.04013392414</v>
       </c>
       <c r="E2">
-        <v>48068.34332341465</v>
+        <v>48141.63465968824</v>
       </c>
       <c r="F2">
-        <v>47911.71308275465</v>
+        <v>47983.5575689352</v>
       </c>
       <c r="G2">
-        <v>47752.75231687359</v>
+        <v>47823.14675099129</v>
       </c>
       <c r="H2">
-        <v>47593.29640933009</v>
+        <v>47662.24007211855</v>
       </c>
       <c r="I2">
-        <v>47433.51664250958</v>
+        <v>47501.00937056764</v>
       </c>
       <c r="J2">
-        <v>47273.66940253328</v>
+        <v>47339.71115130379</v>
       </c>
       <c r="K2">
-        <v>47129.69388079088</v>
+        <v>47194.28465123341</v>
       </c>
       <c r="L2">
-        <v>47006.42030478049</v>
+        <v>47069.56005917418</v>
       </c>
       <c r="M2">
-        <v>46883.10179474726</v>
+        <v>46944.79058654243</v>
       </c>
       <c r="N2">
-        <v>46760.08942476291</v>
+        <v>46820.32708690343</v>
       </c>
       <c r="O2">
-        <v>46638.11875172527</v>
+        <v>46696.90552880164</v>
       </c>
       <c r="P2">
-        <v>46513.05595683573</v>
+        <v>46570.39172335657</v>
       </c>
       <c r="Q2">
-        <v>46389.81722572374</v>
+        <v>46445.70196204122</v>
       </c>
       <c r="R2">
-        <v>46266.23508610406</v>
+        <v>46320.66841128656</v>
       </c>
       <c r="S2">
-        <v>46142.51980473923</v>
+        <v>46195.5023119673</v>
       </c>
       <c r="T2">
-        <v>46019.19525628473</v>
+        <v>46070.72671996498</v>
       </c>
       <c r="U2">
-        <v>45895.49509685064</v>
+        <v>45945.57535113927</v>
       </c>
       <c r="V2">
-        <v>45772.06520466444</v>
+        <v>45820.69412449987</v>
       </c>
       <c r="W2">
-        <v>45648.59216441498</v>
+        <v>45695.76957236964</v>
       </c>
       <c r="X2">
-        <v>45518.71700158974</v>
+        <v>45564.03555177029</v>
       </c>
       <c r="Y2">
-        <v>45341.40523801328</v>
+        <v>45385.58365478595</v>
       </c>
       <c r="Z2">
-        <v>45256.88200090573</v>
+        <v>45299.29641873537</v>
       </c>
       <c r="AA2">
-        <v>45094.76147274366</v>
+        <v>45136.0359182326</v>
       </c>
       <c r="AB2">
-        <v>45006.82503002383</v>
+        <v>45046.33741565012</v>
       </c>
       <c r="AC2">
-        <v>44843.27333916345</v>
+        <v>44881.64582077137</v>
       </c>
       <c r="AD2">
-        <v>44758.44608424916</v>
+        <v>44795.05640475154</v>
       </c>
       <c r="AE2">
-        <v>44589.29873543018</v>
+        <v>44624.45135702083</v>
       </c>
       <c r="AF2">
-        <v>44463.43347974552</v>
+        <v>44497.13484405542</v>
       </c>
       <c r="AG2">
-        <v>44338.98579708959</v>
+        <v>44371.23641357909</v>
       </c>
       <c r="AH2">
-        <v>44214.59606624622</v>
+        <v>44245.39569354206</v>
       </c>
       <c r="AI2">
-        <v>44089.97561238195</v>
+        <v>44119.32423601466</v>
       </c>
       <c r="AJ2">
-        <v>43966.27509039073</v>
+        <v>43994.17239761062</v>
       </c>
       <c r="AK2">
-        <v>43841.41889155246</v>
+        <v>43867.86557985593</v>
       </c>
       <c r="AL2">
-        <v>43716.63070769345</v>
+        <v>43741.62639568256</v>
       </c>
       <c r="AM2">
-        <v>43591.60061081677</v>
+        <v>43615.14520565924</v>
       </c>
       <c r="AN2">
-        <v>43467.67591141581</v>
+        <v>43489.76968020611</v>
       </c>
       <c r="AO2">
-        <v>43346.92727946693</v>
+        <v>43367.5701425345</v>
       </c>
     </row>
   </sheetData>
@@ -2587,124 +2587,124 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>208662.0215360806</v>
+        <v>208584.8518200926</v>
       </c>
       <c r="C2">
-        <v>216594.1324752712</v>
+        <v>216518.0395452966</v>
       </c>
       <c r="D2">
-        <v>225460.3885001453</v>
+        <v>225385.6647418447</v>
       </c>
       <c r="E2">
-        <v>234505.1665381879</v>
+        <v>234431.8752019143</v>
       </c>
       <c r="F2">
-        <v>243590.4179296775</v>
+        <v>243518.5734434969</v>
       </c>
       <c r="G2">
-        <v>252684.88486674</v>
+        <v>252614.4904326223</v>
       </c>
       <c r="H2">
-        <v>261781.3881604735</v>
+        <v>261712.444497685</v>
       </c>
       <c r="I2">
-        <v>270878.5504160699</v>
+        <v>270811.0576880118</v>
       </c>
       <c r="J2">
-        <v>279975.8535505889</v>
+        <v>279909.8118018184</v>
       </c>
       <c r="K2">
-        <v>287723.9215047269</v>
+        <v>287659.3307342844</v>
       </c>
       <c r="L2">
-        <v>293714.2444634413</v>
+        <v>293651.1047090475</v>
       </c>
       <c r="M2">
-        <v>299704.6302118303</v>
+        <v>299642.9414200351</v>
       </c>
       <c r="N2">
-        <v>305694.5713698369</v>
+        <v>305634.3337076965</v>
       </c>
       <c r="O2">
-        <v>311683.8632374228</v>
+        <v>311625.0764603463</v>
       </c>
       <c r="P2">
-        <v>317676.1124845382</v>
+        <v>317618.7767180174</v>
       </c>
       <c r="Q2">
-        <v>323666.6916279707</v>
+        <v>323610.8068916533</v>
       </c>
       <c r="R2">
-        <v>329656.8921977612</v>
+        <v>329602.4588725787</v>
       </c>
       <c r="S2">
-        <v>335648.2350935183</v>
+        <v>335595.2525862902</v>
       </c>
       <c r="T2">
-        <v>341638.8689750943</v>
+        <v>341587.3375114141</v>
       </c>
       <c r="U2">
-        <v>347629.6808142329</v>
+        <v>347579.6005599443</v>
       </c>
       <c r="V2">
-        <v>353620.0803940646</v>
+        <v>353571.4514742292</v>
       </c>
       <c r="W2">
-        <v>359610.3148368226</v>
+        <v>359563.1374288679</v>
       </c>
       <c r="X2">
-        <v>365669.3311090611</v>
+        <v>365624.0125588806</v>
       </c>
       <c r="Y2">
-        <v>371672.015361196</v>
+        <v>371627.8369444234</v>
       </c>
       <c r="Z2">
-        <v>377667.0407286889</v>
+        <v>377624.6263108593</v>
       </c>
       <c r="AA2">
-        <v>383650.9848335387</v>
+        <v>383609.7103880498</v>
       </c>
       <c r="AB2">
-        <v>389652.5958579102</v>
+        <v>389613.0834722839</v>
       </c>
       <c r="AC2">
-        <v>395638.1076685023</v>
+        <v>395599.7351868943</v>
       </c>
       <c r="AD2">
-        <v>401636.5297838277</v>
+        <v>401599.9194633254</v>
       </c>
       <c r="AE2">
-        <v>407675.3291663663</v>
+        <v>407640.1765447756</v>
       </c>
       <c r="AF2">
-        <v>413669.0521754132</v>
+        <v>413635.3508111034</v>
       </c>
       <c r="AG2">
-        <v>419661.8584909541</v>
+        <v>419629.6078744646</v>
       </c>
       <c r="AH2">
-        <v>425654.2472760906</v>
+        <v>425623.4476487947</v>
       </c>
       <c r="AI2">
-        <v>431646.8845717858</v>
+        <v>431617.5359481531</v>
       </c>
       <c r="AJ2">
-        <v>437638.0220451694</v>
+        <v>437610.1247379495</v>
       </c>
       <c r="AK2">
-        <v>443631.615274828</v>
+        <v>443605.1685865246</v>
       </c>
       <c r="AL2">
-        <v>449624.4417289363</v>
+        <v>449599.4460409472</v>
       </c>
       <c r="AM2">
-        <v>455617.3735371919</v>
+        <v>455593.8289423496</v>
       </c>
       <c r="AN2">
-        <v>461593.6442268965</v>
+        <v>461571.5504581062</v>
       </c>
       <c r="AO2">
-        <v>467135.3911212894</v>
+        <v>467114.7482582218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>